<commit_message>
Completed Adding a Workbook Password
</commit_message>
<xml_diff>
--- a/28 - Protecting Worksheets and Workbooks/Excel103-AdvancedExercises.xlsx
+++ b/28 - Protecting Worksheets and Workbooks/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/28 - Protecting Worksheets and Workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1570" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1320BB39-FABB-4293-917E-85D2F32E794F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -5420,8 +5420,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -5449,8 +5449,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>

</xml_diff>